<commit_message>
books for December voting update
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Title</t>
   </si>
@@ -38,31 +38,22 @@
     <t>Cover</t>
   </si>
   <si>
-    <t>V E Schwab</t>
-  </si>
-  <si>
-    <t>The Invisible Life of Addie LaRue</t>
-  </si>
-  <si>
-    <t>https://m.media-amazon.com/images/I/71TFsG7r32L._UF894,1000_QL80_.jpg</t>
-  </si>
-  <si>
-    <t>Sabaa Tahir</t>
-  </si>
-  <si>
-    <t>Heir</t>
-  </si>
-  <si>
-    <t>https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1708009510l/206780522.jpg</t>
-  </si>
-  <si>
-    <t>Cassandra Clare</t>
-  </si>
-  <si>
-    <t>Clockwork Angel</t>
-  </si>
-  <si>
-    <t>https://m.media-amazon.com/images/I/8163yn9JujL._UF1000,1000_QL80_.jpg</t>
+    <t>Stacia Stark</t>
+  </si>
+  <si>
+    <t>A Court this Cruel and Lovely</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81JQPNhk3wL._UF1000,1000_QL80_.jpg</t>
+  </si>
+  <si>
+    <t>Kylie Snow</t>
+  </si>
+  <si>
+    <t>The Lies of Lena</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/208884873-the-lies-of-lena</t>
   </si>
   <si>
     <t>Dani Francis</t>
@@ -74,30 +65,6 @@
     <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1728609987i/217245572.jpg</t>
   </si>
   <si>
-    <t>Amanda Bouchet</t>
-  </si>
-  <si>
-    <t>A Promise of Fire</t>
-  </si>
-  <si>
-    <t>https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1637182295i/59645282.jpg</t>
-  </si>
-  <si>
-    <t>S.T. Gibson</t>
-  </si>
-  <si>
-    <t>A Dowry of Blood</t>
-  </si>
-  <si>
-    <t>https://m.media-amazon.com/images/I/71vVKwhIkyL._UF1000,1000_QL80_.jpg</t>
-  </si>
-  <si>
-    <t>City of Bones</t>
-  </si>
-  <si>
-    <t>https://m.media-amazon.com/images/I/81tUWpvsV9L._UF894,1000_QL80_.jpg</t>
-  </si>
-  <si>
     <t>Rebecca Robinson</t>
   </si>
   <si>
@@ -116,13 +83,13 @@
     <t>https://devneyperry.com/wp-content/uploads/2024/11/ShieldOfSparrows-1600-1.jpg</t>
   </si>
   <si>
-    <t>James Islington</t>
-  </si>
-  <si>
-    <t>The Will of the Many</t>
-  </si>
-  <si>
-    <t>https://m.media-amazon.com/images/S/compressed.photo.goodreads.com/books/1670363463i/58416952.jpg</t>
+    <t>Ali Hazelwood</t>
+  </si>
+  <si>
+    <t>Bound</t>
+  </si>
+  <si>
+    <t>https://alihazelwood.com/wp-content/uploads/2025/09/Bound_final-cover-1280x1280.jpg</t>
   </si>
   <si>
     <t>Hazel McBride</t>
@@ -161,13 +128,64 @@
     <t>https://m.media-amazon.com/images/I/81XCo+49lBL._AC_UF894,1000_QL80_.jpg</t>
   </si>
   <si>
-    <t>Stephanie Garber</t>
-  </si>
-  <si>
-    <t>Alchemy of Secrets</t>
-  </si>
-  <si>
-    <t>https://media.s-bol.com/o46xGAZXkOZ3/pg2K7JV/546x840.jpg</t>
+    <t>Laura Steven</t>
+  </si>
+  <si>
+    <t>Our Infinite Fates</t>
+  </si>
+  <si>
+    <t>https://media.s-bol.com/qqpx7R9N41vy/zpzk5BZ/539x840.jpg</t>
+  </si>
+  <si>
+    <t>Invi Wright</t>
+  </si>
+  <si>
+    <t>The Female</t>
+  </si>
+  <si>
+    <t>https://api.bruna.nl/images/active/carrousel/fullsize/9781966285007_front.jpg</t>
+  </si>
+  <si>
+    <t>Bride</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/228256271-mate</t>
+  </si>
+  <si>
+    <t>Erin Sterling</t>
+  </si>
+  <si>
+    <t>The Ex Hex</t>
+  </si>
+  <si>
+    <t>https://www.goodreads.com/book/show/56554626-the-ex-hex</t>
+  </si>
+  <si>
+    <t>RuNyx</t>
+  </si>
+  <si>
+    <t>Enigma</t>
+  </si>
+  <si>
+    <t>https://mpd-biblio-covers.imgix.net/9781250334244.jpg?w=300&amp;dpr=3</t>
+  </si>
+  <si>
+    <t>Sangu Mandanna</t>
+  </si>
+  <si>
+    <t>A witch's guide to magical innkeeping</t>
+  </si>
+  <si>
+    <t>https://m.media-amazon.com/images/I/81dAeVEo8ML._UF1000,1000_QL80_.jpg</t>
+  </si>
+  <si>
+    <t>Thea Guanzon</t>
+  </si>
+  <si>
+    <t>Tusk Love</t>
+  </si>
+  <si>
+    <t>https://i0.wp.com/thenerddaily.com/wp-content/uploads/2025/07/Tusk-Love-by-Thea-Guanzon.jpg?w=964&amp;ssl=1</t>
   </si>
 </sst>
 </file>
@@ -212,11 +230,10 @@
     <font>
       <sz val="10"/>
       <color rgb="FF1E1915"/>
-      <name val="Copernicus"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="10"/>
       <color rgb="FF1E1915"/>
       <name val="Copernicus"/>
@@ -865,7 +882,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1390,10 +1407,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F12" sqref="F11:F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -1425,18 +1442,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" ht="53.55" spans="1:3">
+    <row r="3" ht="27.15" spans="1:3">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" ht="40.35" spans="1:3">
+    <row r="4" ht="53.55" spans="1:3">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -1447,7 +1464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" ht="53.55" spans="1:3">
+    <row r="5" ht="40.35" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -1458,7 +1475,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" ht="53.55" spans="1:3">
+    <row r="6" ht="40.35" spans="1:3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -1482,73 +1499,73 @@
     </row>
     <row r="8" ht="40.35" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="B8" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="9" ht="40.35" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" ht="40.35" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" ht="53.55" spans="1:3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" ht="40.35" spans="1:3">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" ht="40.35" spans="1:3">
       <c r="A12" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" ht="40.35" spans="1:3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" ht="27.15" spans="1:3">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" ht="40.35" spans="1:3">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" ht="27.15" spans="1:3">
       <c r="A14" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>39</v>
@@ -1557,11 +1574,11 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" ht="40.35" spans="1:3">
+    <row r="15" ht="27.15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1579,23 +1596,47 @@
         <v>46</v>
       </c>
     </row>
+    <row r="17" ht="40.35" spans="1:3">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" ht="40.35" spans="1:3">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="https://m.media-amazon.com/images/I/71TFsG7r32L._UF894,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/71TFsG7r32L._UF894,1000_QL80_.jpg"/>
-    <hyperlink ref="C3" r:id="rId2" display="https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1708009510l/206780522.jpg" tooltip="https://i.gr-assets.com/images/S/compressed.photo.goodreads.com/books/1708009510l/206780522.jpg"/>
-    <hyperlink ref="C4" r:id="rId3" display="https://m.media-amazon.com/images/I/8163yn9JujL._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/8163yn9JujL._UF1000,1000_QL80_.jpg"/>
-    <hyperlink ref="C5" r:id="rId4" display="https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1728609987i/217245572.jpg" tooltip="https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1728609987i/217245572.jpg"/>
-    <hyperlink ref="C6" r:id="rId5" display="https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1637182295i/59645282.jpg" tooltip="https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1637182295i/59645282.jpg"/>
-    <hyperlink ref="C7" r:id="rId6" display="https://m.media-amazon.com/images/I/71vVKwhIkyL._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/71vVKwhIkyL._UF1000,1000_QL80_.jpg"/>
-    <hyperlink ref="C8" r:id="rId7" display="https://m.media-amazon.com/images/I/81tUWpvsV9L._UF894,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/81tUWpvsV9L._UF894,1000_QL80_.jpg"/>
-    <hyperlink ref="C9" r:id="rId8" display="https://m.media-amazon.com/images/I/7186YNOq9wL._SY466_.jpg" tooltip="https://m.media-amazon.com/images/I/7186YNOq9wL._SY466_.jpg"/>
-    <hyperlink ref="C10" r:id="rId9" display="https://devneyperry.com/wp-content/uploads/2024/11/ShieldOfSparrows-1600-1.jpg" tooltip="https://devneyperry.com/wp-content/uploads/2024/11/ShieldOfSparrows-1600-1.jpg"/>
-    <hyperlink ref="C11" r:id="rId10" display="https://m.media-amazon.com/images/S/compressed.photo.goodreads.com/books/1670363463i/58416952.jpg" tooltip="https://m.media-amazon.com/images/S/compressed.photo.goodreads.com/books/1670363463i/58416952.jpg"/>
-    <hyperlink ref="C12" r:id="rId11" display="https://m.media-amazon.com/images/I/91E0OEUccOL._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/91E0OEUccOL._UF1000,1000_QL80_.jpg"/>
-    <hyperlink ref="C13" r:id="rId12" display="https://media.s-bol.com/JkE8nB1gOpr9/mZ8qPNp/546x840.jpg" tooltip="https://media.s-bol.com/JkE8nB1gOpr9/mZ8qPNp/546x840.jpg"/>
-    <hyperlink ref="C14" r:id="rId13" display="https://m.media-amazon.com/images/I/81YOu17CxTL._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/81YOu17CxTL._UF1000,1000_QL80_.jpg"/>
-    <hyperlink ref="C15" r:id="rId14" display="https://m.media-amazon.com/images/I/81XCo+49lBL._AC_UF894,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/81XCo+49lBL._AC_UF894,1000_QL80_.jpg"/>
-    <hyperlink ref="C16" r:id="rId15" display="https://media.s-bol.com/o46xGAZXkOZ3/pg2K7JV/546x840.jpg" tooltip="https://media.s-bol.com/o46xGAZXkOZ3/pg2K7JV/546x840.jpg"/>
+    <hyperlink ref="C2" r:id="rId1" display="https://m.media-amazon.com/images/I/81JQPNhk3wL._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/81JQPNhk3wL._UF1000,1000_QL80_.jpg"/>
+    <hyperlink ref="C3" r:id="rId2" display="https://www.goodreads.com/book/show/208884873-the-lies-of-lena" tooltip="https://www.goodreads.com/book/show/208884873-the-lies-of-lena"/>
+    <hyperlink ref="C4" r:id="rId3" display="https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1728609987i/217245572.jpg" tooltip="https://images-na.ssl-images-amazon.com/images/S/compressed.photo.goodreads.com/books/1728609987i/217245572.jpg"/>
+    <hyperlink ref="C5" r:id="rId4" display="https://m.media-amazon.com/images/I/7186YNOq9wL._SY466_.jpg" tooltip="https://m.media-amazon.com/images/I/7186YNOq9wL._SY466_.jpg"/>
+    <hyperlink ref="C6" r:id="rId5" display="https://devneyperry.com/wp-content/uploads/2024/11/ShieldOfSparrows-1600-1.jpg" tooltip="https://devneyperry.com/wp-content/uploads/2024/11/ShieldOfSparrows-1600-1.jpg"/>
+    <hyperlink ref="C7" r:id="rId6" display="https://alihazelwood.com/wp-content/uploads/2025/09/Bound_final-cover-1280x1280.jpg" tooltip="https://alihazelwood.com/wp-content/uploads/2025/09/Bound_final-cover-1280x1280.jpg"/>
+    <hyperlink ref="C8" r:id="rId7" display="https://m.media-amazon.com/images/I/91E0OEUccOL._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/91E0OEUccOL._UF1000,1000_QL80_.jpg"/>
+    <hyperlink ref="C9" r:id="rId8" display="https://media.s-bol.com/JkE8nB1gOpr9/mZ8qPNp/546x840.jpg" tooltip="https://media.s-bol.com/JkE8nB1gOpr9/mZ8qPNp/546x840.jpg"/>
+    <hyperlink ref="C10" r:id="rId9" display="https://m.media-amazon.com/images/I/81YOu17CxTL._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/81YOu17CxTL._UF1000,1000_QL80_.jpg"/>
+    <hyperlink ref="C11" r:id="rId10" display="https://m.media-amazon.com/images/I/81XCo+49lBL._AC_UF894,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/81XCo+49lBL._AC_UF894,1000_QL80_.jpg"/>
+    <hyperlink ref="C12" r:id="rId11" display="https://media.s-bol.com/qqpx7R9N41vy/zpzk5BZ/539x840.jpg" tooltip="https://media.s-bol.com/qqpx7R9N41vy/zpzk5BZ/539x840.jpg"/>
+    <hyperlink ref="C13" r:id="rId12" display="https://api.bruna.nl/images/active/carrousel/fullsize/9781966285007_front.jpg" tooltip="https://api.bruna.nl/images/active/carrousel/fullsize/9781966285007_front.jpg"/>
+    <hyperlink ref="C14" r:id="rId13" display="https://www.goodreads.com/book/show/228256271-mate" tooltip="https://www.goodreads.com/book/show/228256271-mate"/>
+    <hyperlink ref="C15" r:id="rId14" display="https://www.goodreads.com/book/show/56554626-the-ex-hex" tooltip="https://www.goodreads.com/book/show/56554626-the-ex-hex"/>
+    <hyperlink ref="C16" r:id="rId15" display="https://mpd-biblio-covers.imgix.net/9781250334244.jpg?w=300&amp;dpr=3" tooltip="https://mpd-biblio-covers.imgix.net/9781250334244.jpg?w=300&amp;dpr=3"/>
+    <hyperlink ref="C17" r:id="rId16" display="https://m.media-amazon.com/images/I/81dAeVEo8ML._UF1000,1000_QL80_.jpg" tooltip="https://m.media-amazon.com/images/I/81dAeVEo8ML._UF1000,1000_QL80_.jpg"/>
+    <hyperlink ref="C18" r:id="rId17" display="https://i0.wp.com/thenerddaily.com/wp-content/uploads/2025/07/Tusk-Love-by-Thea-Guanzon.jpg?w=964&amp;ssl=1" tooltip="https://i0.wp.com/thenerddaily.com/wp-content/uploads/2025/07/Tusk-Love-by-Thea-Guanzon.jpg?w=964&amp;ssl=1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>